<commit_message>
modify air-condition control logics
</commit_message>
<xml_diff>
--- a/air_condition/docs/张先生  0310.xlsx
+++ b/air_condition/docs/张先生  0310.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="21000" windowHeight="8555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="248">
   <si>
     <t>封装</t>
   </si>
@@ -760,12 +760,6 @@
   </si>
   <si>
     <t>税钱</t>
-  </si>
-  <si>
-    <t>FDWS86068-F085</t>
-  </si>
-  <si>
-    <t>BSC070N10NS</t>
   </si>
 </sst>
 </file>
@@ -774,11 +768,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -815,18 +809,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3C3C3C"/>
-      <name val="Tahoma"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -837,8 +823,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -851,32 +921,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -891,55 +938,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -951,25 +953,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -982,7 +969,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,7 +981,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,67 +1119,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,60 +1137,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1150,19 +1149,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1225,36 +1212,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1292,6 +1259,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1299,16 +1286,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1317,152 +1304,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1530,9 +1517,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1662,7 +1646,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>153035</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1681,7 +1665,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9428480" y="17468850"/>
-          <a:ext cx="2212340" cy="1753870"/>
+          <a:ext cx="2212340" cy="1570990"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2071,10 +2055,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P108"/>
+  <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2105,16 +2089,16 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5">
@@ -2129,16 +2113,16 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="5">
@@ -2153,16 +2137,16 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="5">
@@ -2183,10 +2167,10 @@
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5">
@@ -2201,16 +2185,16 @@
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="7">
@@ -2282,16 +2266,16 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="5">
@@ -2306,16 +2290,16 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="5">
@@ -2330,16 +2314,16 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="5">
@@ -2354,16 +2338,16 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="5">
@@ -2378,16 +2362,16 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="5">
@@ -2402,16 +2386,16 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="5">
@@ -2426,16 +2410,16 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="5">
@@ -2450,16 +2434,16 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>52</v>
       </c>
       <c r="E16" s="5">
@@ -2507,7 +2491,7 @@
       <c r="C18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>59</v>
       </c>
       <c r="E18" s="5">
@@ -2528,10 +2512,10 @@
       <c r="B19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="5">
@@ -2546,16 +2530,16 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="5">
@@ -2570,16 +2554,16 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="23" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="5">
@@ -2594,16 +2578,16 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="23" t="s">
         <v>69</v>
       </c>
       <c r="E22" s="5">
@@ -2618,16 +2602,16 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="23" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="5">
@@ -2642,16 +2626,16 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>73</v>
       </c>
       <c r="E24" s="5">
@@ -2666,16 +2650,16 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="23" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="5">
@@ -2690,16 +2674,16 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>77</v>
       </c>
       <c r="E26" s="5">
@@ -2714,16 +2698,16 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="23" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="5">
@@ -2738,16 +2722,16 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="23" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="5">
@@ -2762,16 +2746,16 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="23" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="5">
@@ -2786,16 +2770,16 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="23" t="s">
         <v>85</v>
       </c>
       <c r="E30" s="5">
@@ -2810,16 +2794,16 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="23" t="s">
         <v>87</v>
       </c>
       <c r="E31" s="5">
@@ -2834,16 +2818,16 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="23" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="5">
@@ -2858,16 +2842,16 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="23" t="s">
         <v>91</v>
       </c>
       <c r="E33" s="5">
@@ -2882,16 +2866,16 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="23" t="s">
         <v>93</v>
       </c>
       <c r="E34" s="5">
@@ -2906,16 +2890,16 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="23" t="s">
         <v>95</v>
       </c>
       <c r="E35" s="5">
@@ -2930,16 +2914,16 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="23" t="s">
         <v>97</v>
       </c>
       <c r="E36" s="5">
@@ -2954,16 +2938,16 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="23" t="s">
         <v>99</v>
       </c>
       <c r="E37" s="5">
@@ -3122,16 +3106,16 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="23" t="s">
         <v>110</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="23" t="s">
         <v>113</v>
       </c>
       <c r="E44" s="5">
@@ -3152,10 +3136,10 @@
       <c r="B45" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="23" t="s">
         <v>115</v>
       </c>
       <c r="E45" s="5">
@@ -3170,16 +3154,16 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D46" s="23" t="s">
         <v>118</v>
       </c>
       <c r="E46" s="5">
@@ -3194,16 +3178,16 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="23" t="s">
         <v>119</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D47" s="23" t="s">
         <v>121</v>
       </c>
       <c r="E47" s="5">
@@ -3242,16 +3226,16 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="23" t="s">
         <v>127</v>
       </c>
       <c r="E49" s="5">
@@ -3266,16 +3250,16 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D50" s="24" t="s">
+      <c r="D50" s="23" t="s">
         <v>129</v>
       </c>
       <c r="E50" s="5">
@@ -3290,16 +3274,16 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D51" s="23" t="s">
         <v>131</v>
       </c>
       <c r="E51" s="5">
@@ -3314,7 +3298,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="23" t="s">
         <v>132</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -3323,7 +3307,7 @@
       <c r="C52" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="23" t="s">
         <v>135</v>
       </c>
       <c r="E52" s="5">
@@ -3338,16 +3322,16 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="23" t="s">
         <v>136</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D53" s="23" t="s">
         <v>138</v>
       </c>
       <c r="E53" s="5">
@@ -3362,7 +3346,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="23" t="s">
         <v>139</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -3371,7 +3355,7 @@
       <c r="C54" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="23" t="s">
         <v>141</v>
       </c>
       <c r="E54" s="5">
@@ -3386,7 +3370,7 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="23" t="s">
         <v>142</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -3395,7 +3379,7 @@
       <c r="C55" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D55" s="23" t="s">
         <v>144</v>
       </c>
       <c r="E55" s="5">
@@ -3410,7 +3394,7 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="23" t="s">
         <v>145</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -3419,7 +3403,7 @@
       <c r="C56" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="23" t="s">
         <v>147</v>
       </c>
       <c r="E56" s="5">
@@ -3434,7 +3418,7 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>148</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -3443,7 +3427,7 @@
       <c r="C57" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="24" t="s">
+      <c r="D57" s="23" t="s">
         <v>150</v>
       </c>
       <c r="E57" s="5">
@@ -3530,16 +3514,16 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="23" t="s">
         <v>161</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C61" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D61" s="23" t="s">
         <v>164</v>
       </c>
       <c r="E61" s="5">
@@ -3554,16 +3538,16 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="23" t="s">
         <v>165</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D62" s="23" t="s">
         <v>168</v>
       </c>
       <c r="E62" s="5">
@@ -3578,16 +3562,16 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="23" t="s">
         <v>169</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D63" s="23" t="s">
         <v>172</v>
       </c>
       <c r="E63" s="5">
@@ -3602,16 +3586,16 @@
       </c>
     </row>
     <row r="64" ht="28.8" spans="1:7">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="23" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D64" s="23" t="s">
         <v>174</v>
       </c>
       <c r="E64" s="5">
@@ -3626,16 +3610,16 @@
       </c>
     </row>
     <row r="65" ht="28.8" spans="1:7">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="23" t="s">
         <v>169</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="24" t="s">
+      <c r="D65" s="23" t="s">
         <v>176</v>
       </c>
       <c r="E65" s="5">
@@ -3650,16 +3634,16 @@
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="D66" s="24" t="s">
+      <c r="D66" s="23" t="s">
         <v>179</v>
       </c>
       <c r="E66" s="5">
@@ -3674,16 +3658,16 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D67" s="24" t="s">
+      <c r="D67" s="23" t="s">
         <v>181</v>
       </c>
       <c r="E67" s="5">
@@ -3698,16 +3682,16 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="23" t="s">
         <v>183</v>
       </c>
       <c r="E68" s="5">
@@ -3722,16 +3706,16 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D69" s="24" t="s">
+      <c r="D69" s="23" t="s">
         <v>185</v>
       </c>
       <c r="E69" s="5">
@@ -3746,16 +3730,16 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="24" t="s">
+      <c r="A70" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="24" t="s">
+      <c r="D70" s="23" t="s">
         <v>187</v>
       </c>
       <c r="E70" s="5">
@@ -3770,16 +3754,16 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="23" t="s">
         <v>189</v>
       </c>
       <c r="E71" s="5">
@@ -3794,16 +3778,16 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D72" s="23" t="s">
         <v>191</v>
       </c>
       <c r="E72" s="5">
@@ -3818,16 +3802,16 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="24" t="s">
+      <c r="A73" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="D73" s="24" t="s">
+      <c r="D73" s="23" t="s">
         <v>193</v>
       </c>
       <c r="E73" s="5">
@@ -3842,16 +3826,16 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="D74" s="24" t="s">
+      <c r="D74" s="23" t="s">
         <v>195</v>
       </c>
       <c r="E74" s="5">
@@ -3866,16 +3850,16 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="24" t="s">
+      <c r="A75" s="23" t="s">
         <v>196</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="D75" s="24" t="s">
+      <c r="D75" s="23" t="s">
         <v>198</v>
       </c>
       <c r="E75" s="5">
@@ -3992,10 +3976,10 @@
       <c r="B80" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="D80" s="24" t="s">
+      <c r="D80" s="23" t="s">
         <v>212</v>
       </c>
       <c r="E80" s="5">
@@ -4064,10 +4048,10 @@
       <c r="B83" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D83" s="24" t="s">
+      <c r="D83" s="23" t="s">
         <v>220</v>
       </c>
       <c r="E83" s="5">
@@ -4082,16 +4066,16 @@
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="27" t="s">
+      <c r="A84" s="26" t="s">
         <v>221</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="C84" s="27" t="s">
+      <c r="C84" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D84" s="27" t="s">
+      <c r="D84" s="26" t="s">
         <v>223</v>
       </c>
       <c r="E84" s="19">
@@ -4106,16 +4090,16 @@
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="24" t="s">
+      <c r="A85" s="23" t="s">
         <v>224</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="D85" s="24" t="s">
+      <c r="D85" s="23" t="s">
         <v>153</v>
       </c>
       <c r="E85" s="5">
@@ -4130,16 +4114,16 @@
       </c>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="24" t="s">
+      <c r="A86" s="23" t="s">
         <v>226</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="D86" s="24" t="s">
+      <c r="D86" s="23" t="s">
         <v>228</v>
       </c>
       <c r="E86" s="5">
@@ -4154,16 +4138,16 @@
       </c>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="24" t="s">
+      <c r="A87" s="23" t="s">
         <v>229</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="D87" s="24" t="s">
+      <c r="D87" s="23" t="s">
         <v>231</v>
       </c>
       <c r="E87" s="5">
@@ -4356,21 +4340,6 @@
       <c r="G96" s="20">
         <f>SUM(G94:G95)</f>
         <v>1322</v>
-      </c>
-    </row>
-    <row r="106" spans="3:3">
-      <c r="C106" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="107" spans="3:3">
-      <c r="C107" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="108" ht="15" spans="3:3">
-      <c r="C108" s="23" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>